<commit_message>
Jesi: Slit Lamp Final Version (10/29/2020)
</commit_message>
<xml_diff>
--- a/Project Outputs for Slit_Lamp/BOM/Bill of Materials-Slit_Lamp.xlsx
+++ b/Project Outputs for Slit_Lamp/BOM/Bill of Materials-Slit_Lamp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Slit_Lamp\Project Outputs for Slit_Lamp\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{092CBD13-75FD-4D1F-939A-25B75E6D586E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9227220-CF40-4D33-88CA-E4DD7961A7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14142" yWindow="432" windowWidth="8748" windowHeight="11928" xr2:uid="{EB0E2B69-B176-4E7D-B1BD-89339549538B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{278AC516-F53A-4BD1-AEAF-A3092695D8F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Slit_Lamp" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
   <si>
     <t>Comment</t>
   </si>
@@ -71,7 +72,7 @@
     <t>10K resistor</t>
   </si>
   <si>
-    <t>10k, LIMIT_R, SLIT_BUT_R</t>
+    <t>10k, LIMIT_R, RESET_BUT_R, SLIT_BUT_R</t>
   </si>
   <si>
     <t>Vishay</t>
@@ -92,22 +93,23 @@
     <t>CONN 3 Positions Header, Shrouded Connector 0.039" (1.00mm) Surface Mount Tin</t>
   </si>
   <si>
-    <t>Buttons connector</t>
+    <t>Buttons connector, Current driver input, Potentiometer1</t>
   </si>
   <si>
     <t>JST</t>
   </si>
   <si>
-    <t>Arrow</t>
+    <t>Arrow Electronics</t>
   </si>
   <si>
     <t>455-1789-1-ND</t>
   </si>
   <si>
-    <t>06031C103K4T2A</t>
-  </si>
-  <si>
-    <t>Capacitor 0.01uF</t>
+    <t>0.01uF</t>
+  </si>
+  <si>
+    <t>Capacitor 0.01uF_x000D_
+06031C103K4T2A</t>
   </si>
   <si>
     <t>C1</t>
@@ -137,97 +139,82 @@
     <t>GRM155R60J475ME47D</t>
   </si>
   <si>
-    <t>0402ZD225MAT2A</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor, Multilayer, Ceramic, 10V, 10% +Tol, 10% -Tol, X5R, 15% TC, 10uF, Surface Mount, 0603</t>
+    <t>Capacitor 10µF +/-40% 6.3V 0402</t>
+  </si>
+  <si>
+    <t>Chip Capacitor, 10µF +/-40%, 6.3V, 0402, Thickness 0.6 mm</t>
   </si>
   <si>
     <t>C3, C5</t>
   </si>
   <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>3581672</t>
+  </si>
+  <si>
+    <t>TDK CGA3E2X7R1H104K080AA</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, 15% TC, 0.1uF, Surface Mount, 0603</t>
+  </si>
+  <si>
+    <t>C4, C6</t>
+  </si>
+  <si>
     <t>TDK</t>
   </si>
   <si>
-    <t>445-7486-1-ND</t>
-  </si>
-  <si>
-    <t>TDK CGA3E2X7R1H104K080AA</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, 15% TC, 0.1uF, Surface Mount, 0603</t>
-  </si>
-  <si>
-    <t>C4, C6</t>
-  </si>
-  <si>
     <t>445-5666-1-ND</t>
   </si>
   <si>
+    <t>JST BM02B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN 2 Positions Header, Shrouded Connector 0.039" (1.00mm) Surface Mount Tin</t>
+  </si>
+  <si>
+    <t>Focus_led, Limit Switch</t>
+  </si>
+  <si>
+    <t>455-1788-1-ND</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>Fixed Resistor, Metal Glaze/thick Film, 0.1W, 1000000ohm, 75V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0603</t>
+  </si>
+  <si>
+    <t>FOCUS_R</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>P1.00MHCT-ND</t>
+  </si>
+  <si>
+    <t>DRV8834RGET</t>
+  </si>
+  <si>
+    <t>Brush DC Motor Controller, 2.2A, PQCC24</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>296-37691-1-ND</t>
+  </si>
+  <si>
     <t>JST BM03B-SRSS-TB(LF)(SN)</t>
   </si>
   <si>
-    <t>Current driver input</t>
-  </si>
-  <si>
-    <t>JST BM02B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>CONN 2 Positions Header, Shrouded Connector 0.039" (1.00mm) Surface Mount Tin</t>
-  </si>
-  <si>
-    <t>Focus_led, Limit Switch</t>
-  </si>
-  <si>
-    <t>455-1788-1-ND</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>Fixed Resistor, Metal Glaze/thick Film, 0.1W, 1000000ohm, 75V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0603</t>
-  </si>
-  <si>
-    <t>FOCUS_R</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>P1.00MHCT-ND</t>
-  </si>
-  <si>
-    <t>DRV8834RGET</t>
-  </si>
-  <si>
-    <t>Brush DC Motor Controller, 2.2A, PQCC24</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>296-37691-1-ND</t>
-  </si>
-  <si>
-    <t>ADAFRUIT_METRO_MINI</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>METRO_MINI</t>
-  </si>
-  <si>
-    <t>ON-OFF-SWITCH, Potentiometer</t>
-  </si>
-  <si>
-    <t>ADAFRUIT_POWER_BOOST</t>
-  </si>
-  <si>
-    <t>POWER_1000C</t>
+    <t>ON-OFF-SWITCH</t>
   </si>
   <si>
     <t>35WR10KLFTR</t>
@@ -242,9 +229,6 @@
     <t xml:space="preserve">TT BI </t>
   </si>
   <si>
-    <t>Farnell</t>
-  </si>
-  <si>
     <t>1420214</t>
   </si>
   <si>
@@ -311,16 +295,13 @@
     <t>541-1.00HCT-ND</t>
   </si>
   <si>
-    <t>RESET_BUT_R</t>
-  </si>
-  <si>
-    <t>BM04B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>Connector Header Surface Mount 4 position 0.039 _1.00mm_</t>
-  </si>
-  <si>
-    <t>Shutters</t>
+    <t>BM04B-SRSS</t>
+  </si>
+  <si>
+    <t>JST SH series header 1.00mm pitch disconnectable crimp style connectors, vertical (side entry type), 4 pins</t>
+  </si>
+  <si>
+    <t>Shutter, STEP_PINS</t>
   </si>
   <si>
     <t>455-1790-1-ND</t>
@@ -336,15 +317,6 @@
   </si>
   <si>
     <t>PCE3783CT-ND</t>
-  </si>
-  <si>
-    <t>O-Br-Bl-R</t>
-  </si>
-  <si>
-    <t>JST SH series header 1.00mm pitch disconnectable crimp style connectors, vertical (side entry type), 4 pins</t>
-  </si>
-  <si>
-    <t>STEP_PINS</t>
   </si>
   <si>
     <t>SN74LS279ADR</t>
@@ -741,10 +713,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A049950-D3BB-48F5-970A-ECF9AD2C1242}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F7227C-4F4C-4B44-BB2F-A78EE4A1A766}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -781,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -792,7 +766,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -821,7 +795,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>19</v>
@@ -839,7 +813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -895,7 +869,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -909,13 +883,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>13</v>
@@ -938,10 +912,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
@@ -950,21 +924,21 @@
         <v>14</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
@@ -976,231 +950,251 @@
         <v>13</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -1209,248 +1203,103 @@
         <v>12</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D18" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="4">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>